<commit_message>
added week 4 training materials
</commit_message>
<xml_diff>
--- a/TOC/2024.Nov.ASDE Training TOC - v4.xlsx
+++ b/TOC/2024.Nov.ASDE Training TOC - v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online Training\ACE\Sapient\PSI-2024 Nov ASDE BLR Batch 1\TOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EB54D5-0B20-4E22-9537-05E4ABBA1B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD29C13F-8EF3-42A1-96A7-B7E98746E710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="599" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="599" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Template - 2022" sheetId="10" r:id="rId1"/>
@@ -18355,7 +18355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A7F07D-A6D7-4BA7-ADA6-D6244D6DC8FA}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
       <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
@@ -18964,9 +18964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E77354-39DB-4E45-A638-0E6F14DE89BD}">
   <dimension ref="A1:M1890"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A933" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C938" sqref="C938"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A1437" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1412" sqref="C1412:C1415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
added week 5 training materials
</commit_message>
<xml_diff>
--- a/TOC/2024.Nov.ASDE Training TOC - v4.xlsx
+++ b/TOC/2024.Nov.ASDE Training TOC - v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online Training\ACE\Sapient\PSI-2024 Nov ASDE BLR Batch 1\TOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD29C13F-8EF3-42A1-96A7-B7E98746E710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69E018C-7FF7-4CB4-B3FA-15AA45A85CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="599" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4746" uniqueCount="2155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4732" uniqueCount="2141">
   <si>
     <t>Topic</t>
   </si>
@@ -6438,111 +6438,6 @@
     <t>Cloud Console</t>
   </si>
   <si>
-    <t>1. Provisioning GKE Cluster</t>
-  </si>
-  <si>
-    <t>1.1 Set Up GCP Environment</t>
-  </si>
-  <si>
-    <t>Install and configure Google Cloud CLI</t>
-  </si>
-  <si>
-    <t>Enable required GCP APIs</t>
-  </si>
-  <si>
-    <t>1.2 Provision GKE Cluster</t>
-  </si>
-  <si>
-    <t>Using gcloud CLI for manual setup</t>
-  </si>
-  <si>
-    <t>1.3 Connect to the Cluster</t>
-  </si>
-  <si>
-    <t>Authenticating kubectl with GKE</t>
-  </si>
-  <si>
-    <t>2. Deployment Pipeline</t>
-  </si>
-  <si>
-    <t>2.1 Create Deployment Pipeline in Jenkins</t>
-  </si>
-  <si>
-    <t>Define Jenkins pipeline steps</t>
-  </si>
-  <si>
-    <t>Integrate Docker and Kubernetes configurations</t>
-  </si>
-  <si>
-    <t>2.2 Set Up Secrets</t>
-  </si>
-  <si>
-    <t>3. Application Deployment</t>
-  </si>
-  <si>
-    <t>3.1 Create Kubernetes Manifests</t>
-  </si>
-  <si>
-    <t>Deployment configuration (deployment.yaml)</t>
-  </si>
-  <si>
-    <t>Service configuration (service.yaml)</t>
-  </si>
-  <si>
-    <t>3.2 Build and Push Docker Image</t>
-  </si>
-  <si>
-    <t>Dockerfile setup</t>
-  </si>
-  <si>
-    <t>3.3 Deploy to GKE</t>
-  </si>
-  <si>
-    <t>4. Monitor and Manage</t>
-  </si>
-  <si>
-    <t>4.1 Monitor Deployment</t>
-  </si>
-  <si>
-    <t>4.2 Scaling</t>
-  </si>
-  <si>
-    <t>4.3 Logging and Alerts</t>
-  </si>
-  <si>
-    <t>Manage secrets in CI/CD tools</t>
-  </si>
-  <si>
-    <t>Store service account credentials securely</t>
-  </si>
-  <si>
-    <t>Push images to Google Container Registry (GCR)</t>
-  </si>
-  <si>
-    <t>Apply Kubernetes manifests with kubectl</t>
-  </si>
-  <si>
-    <t>Verify deployments and services</t>
-  </si>
-  <si>
-    <t>Use kubectl for pod and service status</t>
-  </si>
-  <si>
-    <t>Access GKE dashboards</t>
-  </si>
-  <si>
-    <t>Scale deployments manually and automatically</t>
-  </si>
-  <si>
-    <t>Enable and access Google Cloud Observability for logging, monitoring, and alerting to gain visibility into the GKE cluster.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">** This process will deploy and test a basic React app in the  Kubernetes cluster. </t>
-  </si>
-  <si>
-    <t>Hands-On: GKE - Provisioning, Deployment Pipeline and App Deployment</t>
-  </si>
-  <si>
     <t>Understanding Scattering Read and Gathering Write Operations</t>
   </si>
   <si>
@@ -6796,6 +6691,69 @@
   </si>
   <si>
     <t>7. Using Docker Compose Commands</t>
+  </si>
+  <si>
+    <t>Hands-On: Deploying the Product Management Application on Google Cloud Storage</t>
+  </si>
+  <si>
+    <t>1: Set Up Google Cloud Storage</t>
+  </si>
+  <si>
+    <t>1.1 Create a Google Cloud Project</t>
+  </si>
+  <si>
+    <t>1.2 Create a Storage Bucket</t>
+  </si>
+  <si>
+    <t>2: Prepare Your Application for Static Deployment</t>
+  </si>
+  <si>
+    <t>2.1 Update next.config.js</t>
+  </si>
+  <si>
+    <t>2.2 Build the Static Site</t>
+  </si>
+  <si>
+    <t>3: Upload Files to Google Cloud Storage</t>
+  </si>
+  <si>
+    <t>3.1 Install Google Cloud CLI</t>
+  </si>
+  <si>
+    <t>3.2 Authenticate with Google Cloud</t>
+  </si>
+  <si>
+    <t>3.3 Set Your Project</t>
+  </si>
+  <si>
+    <t>3.4 Upload Files</t>
+  </si>
+  <si>
+    <t>4: Make the Bucket Public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5: Configure the Bucket for Static Hosting </t>
+  </si>
+  <si>
+    <t>6: Test Your Deployment</t>
+  </si>
+  <si>
+    <t>7: Update the Deployment</t>
+  </si>
+  <si>
+    <t>If you make changes to your app:</t>
+  </si>
+  <si>
+    <t>Complete Workflow</t>
+  </si>
+  <si>
+    <t>Commands Overview</t>
+  </si>
+  <si>
+    <t>1. Rebuild the project</t>
+  </si>
+  <si>
+    <t>2. Re-upload the out directory to the bucket</t>
   </si>
 </sst>
 </file>
@@ -7250,7 +7208,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -7510,6 +7468,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -18962,11 +18923,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E77354-39DB-4E45-A638-0E6F14DE89BD}">
-  <dimension ref="A1:M1890"/>
+  <dimension ref="A1:M1879"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A1437" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1412" sqref="C1412:C1415"/>
+      <pane ySplit="2" topLeftCell="A1572" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1873" sqref="D1873"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -20843,7 +20804,7 @@
     <row r="320" spans="1:9" ht="15.5">
       <c r="B320" s="30"/>
       <c r="C320" s="61" t="s">
-        <v>2078</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="321" spans="2:9" ht="15.5">
@@ -20901,7 +20862,7 @@
     <row r="330" spans="2:9" ht="15.5">
       <c r="B330" s="30"/>
       <c r="C330" s="26" t="s">
-        <v>2079</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="331" spans="2:9" ht="15.5">
@@ -24185,7 +24146,7 @@
       <c r="A939" s="34"/>
       <c r="B939" s="25"/>
       <c r="C939" s="28" t="s">
-        <v>2124</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="940" spans="1:3">
@@ -24196,49 +24157,49 @@
       <c r="A941" s="34"/>
       <c r="B941" s="25"/>
       <c r="C941" s="28" t="s">
-        <v>2125</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="942" spans="1:3">
       <c r="A942" s="34"/>
       <c r="B942" s="25"/>
       <c r="C942" s="28" t="s">
-        <v>2126</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="943" spans="1:3">
       <c r="A943" s="34"/>
       <c r="B943" s="25"/>
       <c r="C943" s="28" t="s">
-        <v>2127</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="944" spans="1:3">
       <c r="A944" s="34"/>
       <c r="B944" s="25"/>
       <c r="C944" s="28" t="s">
-        <v>2128</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="945" spans="1:3">
       <c r="A945" s="34"/>
       <c r="B945" s="25"/>
       <c r="C945" s="28" t="s">
-        <v>2129</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="946" spans="1:3">
       <c r="A946" s="34"/>
       <c r="B946" s="25"/>
       <c r="C946" s="28" t="s">
-        <v>2130</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="947" spans="1:3">
       <c r="A947" s="34"/>
       <c r="B947" s="25"/>
       <c r="C947" s="28" t="s">
-        <v>2131</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="948" spans="1:3">
@@ -24249,63 +24210,63 @@
       <c r="A949" s="34"/>
       <c r="B949" s="25"/>
       <c r="C949" s="28" t="s">
-        <v>2132</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="950" spans="1:3">
       <c r="A950" s="34"/>
       <c r="B950" s="25"/>
       <c r="C950" s="28" t="s">
-        <v>2133</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="951" spans="1:3">
       <c r="A951" s="34"/>
       <c r="B951" s="25"/>
       <c r="C951" s="28" t="s">
-        <v>2134</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="952" spans="1:3">
       <c r="A952" s="34"/>
       <c r="B952" s="25"/>
       <c r="C952" s="28" t="s">
-        <v>2135</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="953" spans="1:3">
       <c r="A953" s="34"/>
       <c r="B953" s="25"/>
       <c r="C953" s="28" t="s">
-        <v>2136</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="954" spans="1:3">
       <c r="A954" s="34"/>
       <c r="B954" s="25"/>
       <c r="C954" s="28" t="s">
-        <v>2137</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="955" spans="1:3">
       <c r="A955" s="34"/>
       <c r="B955" s="25"/>
       <c r="C955" s="28" t="s">
-        <v>2138</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="956" spans="1:3">
       <c r="A956" s="34"/>
       <c r="B956" s="25"/>
       <c r="C956" s="28" t="s">
-        <v>2139</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="957" spans="1:3">
       <c r="A957" s="34"/>
       <c r="B957" s="25"/>
       <c r="C957" s="28" t="s">
-        <v>2140</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="958" spans="1:3">
@@ -24316,56 +24277,56 @@
       <c r="A959" s="34"/>
       <c r="B959" s="25"/>
       <c r="C959" s="28" t="s">
-        <v>2141</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="960" spans="1:3">
       <c r="A960" s="34"/>
       <c r="B960" s="25"/>
       <c r="C960" s="28" t="s">
-        <v>2133</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="961" spans="1:3">
       <c r="A961" s="34"/>
       <c r="B961" s="25"/>
       <c r="C961" s="28" t="s">
-        <v>2142</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="962" spans="1:3">
       <c r="A962" s="34"/>
       <c r="B962" s="25"/>
       <c r="C962" s="28" t="s">
-        <v>2143</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="963" spans="1:3">
       <c r="A963" s="34"/>
       <c r="B963" s="25"/>
       <c r="C963" s="28" t="s">
-        <v>2144</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="964" spans="1:3">
       <c r="A964" s="34"/>
       <c r="B964" s="25"/>
       <c r="C964" s="28" t="s">
-        <v>2145</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="965" spans="1:3">
       <c r="A965" s="34"/>
       <c r="B965" s="25"/>
       <c r="C965" s="28" t="s">
-        <v>2146</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="966" spans="1:3">
       <c r="A966" s="34"/>
       <c r="B966" s="25"/>
       <c r="C966" s="28" t="s">
-        <v>2147</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="967" spans="1:3">
@@ -24376,63 +24337,63 @@
       <c r="A968" s="34"/>
       <c r="B968" s="25"/>
       <c r="C968" s="28" t="s">
-        <v>2148</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="969" spans="1:3">
       <c r="A969" s="34"/>
       <c r="B969" s="25"/>
       <c r="C969" s="28" t="s">
-        <v>2133</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="970" spans="1:3">
       <c r="A970" s="34"/>
       <c r="B970" s="25"/>
       <c r="C970" s="28" t="s">
-        <v>2149</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="971" spans="1:3">
       <c r="A971" s="34"/>
       <c r="B971" s="25"/>
       <c r="C971" s="28" t="s">
-        <v>2150</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="972" spans="1:3">
       <c r="A972" s="34"/>
       <c r="B972" s="25"/>
       <c r="C972" s="28" t="s">
-        <v>2151</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="973" spans="1:3">
       <c r="A973" s="34"/>
       <c r="B973" s="25"/>
       <c r="C973" s="28" t="s">
-        <v>2152</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="974" spans="1:3">
       <c r="A974" s="34"/>
       <c r="B974" s="25"/>
       <c r="C974" s="28" t="s">
-        <v>2153</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="975" spans="1:3">
       <c r="A975" s="34"/>
       <c r="B975" s="25"/>
       <c r="C975" s="28" t="s">
-        <v>2154</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="976" spans="1:3">
       <c r="A976" s="34"/>
       <c r="B976" s="25"/>
       <c r="C976" s="28" t="s">
-        <v>2140</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="977" spans="2:3">
@@ -29072,25 +29033,25 @@
     <row r="1786" spans="1:3">
       <c r="A1786" s="40"/>
       <c r="C1786" s="34" t="s">
-        <v>2080</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="1787" spans="1:3">
       <c r="A1787" s="40"/>
       <c r="C1787" s="56" t="s">
-        <v>2081</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="1788" spans="1:3">
       <c r="A1788" s="40"/>
       <c r="C1788" s="56" t="s">
-        <v>2082</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="1789" spans="1:3">
       <c r="A1789" s="40"/>
       <c r="C1789" s="56" t="s">
-        <v>2083</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="1790" spans="1:3">
@@ -29100,43 +29061,43 @@
     <row r="1791" spans="1:3">
       <c r="A1791" s="40"/>
       <c r="C1791" s="34" t="s">
-        <v>2084</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="1792" spans="1:3">
       <c r="A1792" s="40"/>
       <c r="C1792" t="s">
-        <v>2085</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="1793" spans="1:3">
       <c r="A1793" s="40"/>
       <c r="C1793" t="s">
-        <v>2086</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="1794" spans="1:3">
       <c r="A1794" s="40"/>
       <c r="C1794" t="s">
-        <v>2087</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="1795" spans="1:3">
       <c r="A1795" s="40"/>
       <c r="C1795" s="86" t="s">
-        <v>2088</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="1796" spans="1:3">
       <c r="A1796" s="40"/>
       <c r="C1796" t="s">
-        <v>2090</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="1797" spans="1:3">
       <c r="A1797" s="40"/>
       <c r="C1797" t="s">
-        <v>2089</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="1798" spans="1:3">
@@ -29146,7 +29107,7 @@
     <row r="1799" spans="1:3">
       <c r="A1799" s="40"/>
       <c r="C1799" s="86" t="s">
-        <v>2091</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="1800" spans="1:3">
@@ -29156,19 +29117,19 @@
     <row r="1801" spans="1:3">
       <c r="A1801" s="40"/>
       <c r="C1801" s="34" t="s">
-        <v>2092</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="1802" spans="1:3">
       <c r="A1802" s="40"/>
       <c r="C1802" t="s">
-        <v>2093</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="1803" spans="1:3">
       <c r="A1803" s="40"/>
       <c r="C1803" t="s">
-        <v>2094</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="1804" spans="1:3">
@@ -29178,19 +29139,19 @@
     <row r="1805" spans="1:3">
       <c r="A1805" s="40"/>
       <c r="C1805" s="34" t="s">
-        <v>2095</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="1806" spans="1:3">
       <c r="A1806" s="40"/>
       <c r="C1806" t="s">
-        <v>2097</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="1807" spans="1:3">
       <c r="A1807" s="40"/>
       <c r="C1807" t="s">
-        <v>2096</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="1808" spans="1:3">
@@ -29200,7 +29161,7 @@
     <row r="1809" spans="1:3">
       <c r="A1809" s="40"/>
       <c r="C1809" s="34" t="s">
-        <v>2098</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="1810" spans="1:3">
@@ -29210,7 +29171,7 @@
     <row r="1811" spans="1:3">
       <c r="A1811" s="40"/>
       <c r="C1811" s="34" t="s">
-        <v>2099</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="1812" spans="1:3">
@@ -29220,37 +29181,37 @@
     <row r="1813" spans="1:3">
       <c r="A1813" s="40"/>
       <c r="C1813" s="34" t="s">
-        <v>2100</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="1814" spans="1:3">
       <c r="A1814" s="40"/>
       <c r="C1814" t="s">
-        <v>2101</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="1815" spans="1:3">
       <c r="A1815" s="40"/>
       <c r="C1815" t="s">
-        <v>2102</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="1816" spans="1:3">
       <c r="A1816" s="40"/>
       <c r="C1816" t="s">
-        <v>2103</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="1817" spans="1:3">
       <c r="A1817" s="40"/>
       <c r="C1817" t="s">
-        <v>2099</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="1818" spans="1:3">
       <c r="A1818" s="40"/>
       <c r="C1818" t="s">
-        <v>2105</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="1819" spans="1:3">
@@ -29260,25 +29221,25 @@
     <row r="1820" spans="1:3">
       <c r="A1820" s="40"/>
       <c r="C1820" s="34" t="s">
-        <v>2104</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="1821" spans="1:3">
       <c r="A1821" s="40"/>
       <c r="C1821" t="s">
-        <v>2106</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="1822" spans="1:3">
       <c r="A1822" s="40"/>
       <c r="C1822" t="s">
-        <v>2082</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="1823" spans="1:3">
       <c r="A1823" s="40"/>
       <c r="C1823" t="s">
-        <v>2107</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="1824" spans="1:3">
@@ -29288,19 +29249,19 @@
     <row r="1825" spans="1:3">
       <c r="A1825" s="40"/>
       <c r="C1825" s="86" t="s">
-        <v>2099</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="1826" spans="1:3">
       <c r="A1826" s="40"/>
       <c r="C1826" s="86" t="s">
-        <v>2108</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="1827" spans="1:3">
       <c r="A1827" s="40"/>
       <c r="C1827" s="86" t="s">
-        <v>2109</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="1828" spans="1:3">
@@ -29310,7 +29271,7 @@
     <row r="1829" spans="1:3">
       <c r="A1829" s="40"/>
       <c r="C1829" s="86" t="s">
-        <v>2110</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="1830" spans="1:3">
@@ -29319,49 +29280,49 @@
     <row r="1831" spans="1:3">
       <c r="A1831" s="40"/>
       <c r="C1831" s="86" t="s">
-        <v>2111</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="1832" spans="1:3">
       <c r="A1832" s="40"/>
       <c r="C1832" t="s">
-        <v>2112</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="1833" spans="1:3">
       <c r="A1833" s="40"/>
       <c r="C1833" t="s">
-        <v>2113</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="1834" spans="1:3">
       <c r="A1834" s="40"/>
       <c r="C1834" t="s">
-        <v>2114</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="1835" spans="1:3">
       <c r="A1835" s="40"/>
       <c r="C1835" t="s">
-        <v>2115</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="1836" spans="1:3">
       <c r="A1836" s="40"/>
       <c r="C1836" t="s">
-        <v>2116</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="1837" spans="1:3">
       <c r="A1837" s="40"/>
       <c r="C1837" t="s">
-        <v>2117</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="1838" spans="1:3">
       <c r="A1838" s="40"/>
       <c r="C1838" t="s">
-        <v>2080</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="1839" spans="1:3">
@@ -29371,31 +29332,31 @@
     <row r="1840" spans="1:3">
       <c r="A1840" s="40"/>
       <c r="C1840" s="86" t="s">
-        <v>2118</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="1841" spans="1:3">
       <c r="A1841" s="40"/>
       <c r="C1841" t="s">
-        <v>2119</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="1842" spans="1:3">
       <c r="A1842" s="40"/>
       <c r="C1842" t="s">
-        <v>2120</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="1843" spans="1:3">
       <c r="A1843" s="40"/>
       <c r="C1843" t="s">
-        <v>2121</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="1844" spans="1:3">
       <c r="A1844" s="40"/>
       <c r="C1844" t="s">
-        <v>2122</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="1845" spans="1:3">
@@ -29405,7 +29366,7 @@
     <row r="1846" spans="1:3">
       <c r="A1846" s="40"/>
       <c r="C1846" s="86" t="s">
-        <v>2094</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="1847" spans="1:3">
@@ -29415,251 +29376,179 @@
     <row r="1848" spans="1:3">
       <c r="A1848" s="40"/>
       <c r="C1848" s="86" t="s">
-        <v>2123</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="1849" spans="1:3">
       <c r="A1849" s="40"/>
       <c r="C1849" s="86"/>
     </row>
-    <row r="1850" spans="1:3">
+    <row r="1850" spans="1:3" ht="27">
       <c r="A1850" s="40"/>
-      <c r="C1850" s="34" t="s">
-        <v>2077</v>
+      <c r="C1850" s="81" t="s">
+        <v>2120</v>
       </c>
     </row>
     <row r="1851" spans="1:3">
       <c r="A1851" s="40"/>
-      <c r="C1851" s="34" t="s">
-        <v>2043</v>
+      <c r="C1851" s="81" t="s">
+        <v>2121</v>
       </c>
     </row>
     <row r="1852" spans="1:3">
       <c r="A1852" s="40"/>
-      <c r="C1852" s="34" t="s">
-        <v>2044</v>
+      <c r="C1852" s="84" t="s">
+        <v>2122</v>
       </c>
     </row>
     <row r="1853" spans="1:3">
       <c r="A1853" s="40"/>
-      <c r="C1853" s="56" t="s">
-        <v>2045</v>
+      <c r="C1853" s="84" t="s">
+        <v>2123</v>
       </c>
     </row>
     <row r="1854" spans="1:3">
       <c r="A1854" s="40"/>
-      <c r="C1854" s="56" t="s">
-        <v>2046</v>
-      </c>
+      <c r="C1854" s="84"/>
     </row>
     <row r="1855" spans="1:3">
       <c r="A1855" s="40"/>
-      <c r="C1855" s="34" t="s">
-        <v>2047</v>
+      <c r="C1855" s="81" t="s">
+        <v>2124</v>
       </c>
     </row>
     <row r="1856" spans="1:3">
       <c r="A1856" s="40"/>
-      <c r="C1856" s="56" t="s">
-        <v>2048</v>
+      <c r="C1856" s="84" t="s">
+        <v>2125</v>
       </c>
     </row>
     <row r="1857" spans="1:3">
       <c r="A1857" s="40"/>
-      <c r="C1857" s="34" t="s">
-        <v>2049</v>
+      <c r="C1857" s="84" t="s">
+        <v>2126</v>
       </c>
     </row>
     <row r="1858" spans="1:3">
       <c r="A1858" s="40"/>
-      <c r="C1858" s="56" t="s">
-        <v>2050</v>
-      </c>
+      <c r="C1858" s="84"/>
     </row>
     <row r="1859" spans="1:3">
       <c r="A1859" s="40"/>
-      <c r="C1859" s="56"/>
+      <c r="C1859" s="81" t="s">
+        <v>2127</v>
+      </c>
     </row>
     <row r="1860" spans="1:3">
       <c r="A1860" s="40"/>
-      <c r="C1860" s="34" t="s">
-        <v>2051</v>
+      <c r="C1860" s="84" t="s">
+        <v>2128</v>
       </c>
     </row>
     <row r="1861" spans="1:3">
       <c r="A1861" s="40"/>
-      <c r="C1861" s="34" t="s">
-        <v>2052</v>
+      <c r="C1861" s="84" t="s">
+        <v>2129</v>
       </c>
     </row>
     <row r="1862" spans="1:3">
       <c r="A1862" s="40"/>
-      <c r="C1862" s="56" t="s">
-        <v>2053</v>
+      <c r="C1862" s="84" t="s">
+        <v>2130</v>
       </c>
     </row>
     <row r="1863" spans="1:3">
       <c r="A1863" s="40"/>
-      <c r="C1863" s="56" t="s">
-        <v>2054</v>
+      <c r="C1863" s="84" t="s">
+        <v>2131</v>
       </c>
     </row>
     <row r="1864" spans="1:3">
       <c r="A1864" s="40"/>
-      <c r="C1864" s="34" t="s">
-        <v>2055</v>
-      </c>
+      <c r="C1864" s="84"/>
     </row>
     <row r="1865" spans="1:3">
       <c r="A1865" s="40"/>
-      <c r="C1865" s="56" t="s">
-        <v>2067</v>
+      <c r="C1865" s="81" t="s">
+        <v>2132</v>
       </c>
     </row>
     <row r="1866" spans="1:3">
       <c r="A1866" s="40"/>
-      <c r="C1866" s="56" t="s">
-        <v>2068</v>
-      </c>
+      <c r="C1866" s="84"/>
     </row>
     <row r="1867" spans="1:3">
       <c r="A1867" s="40"/>
-      <c r="C1867" s="56"/>
+      <c r="C1867" s="81" t="s">
+        <v>2133</v>
+      </c>
     </row>
     <row r="1868" spans="1:3">
       <c r="A1868" s="40"/>
-      <c r="C1868" s="34" t="s">
-        <v>2056</v>
-      </c>
+      <c r="C1868" s="84"/>
     </row>
     <row r="1869" spans="1:3">
       <c r="A1869" s="40"/>
-      <c r="C1869" s="34" t="s">
-        <v>2057</v>
+      <c r="C1869" s="81" t="s">
+        <v>2134</v>
       </c>
     </row>
     <row r="1870" spans="1:3">
       <c r="A1870" s="40"/>
-      <c r="C1870" s="56" t="s">
-        <v>2058</v>
-      </c>
+      <c r="C1870" s="84"/>
     </row>
     <row r="1871" spans="1:3">
       <c r="A1871" s="40"/>
-      <c r="C1871" s="56" t="s">
-        <v>2059</v>
+      <c r="C1871" s="81" t="s">
+        <v>2135</v>
       </c>
     </row>
     <row r="1872" spans="1:3">
       <c r="A1872" s="40"/>
-      <c r="C1872" s="34" t="s">
-        <v>2060</v>
+      <c r="C1872" s="84" t="s">
+        <v>2136</v>
       </c>
     </row>
     <row r="1873" spans="1:3">
       <c r="A1873" s="40"/>
-      <c r="C1873" s="56" t="s">
-        <v>2061</v>
+      <c r="C1873" s="94" t="s">
+        <v>2139</v>
       </c>
     </row>
     <row r="1874" spans="1:3">
       <c r="A1874" s="40"/>
-      <c r="C1874" s="56" t="s">
-        <v>2069</v>
+      <c r="C1874" s="94" t="s">
+        <v>2140</v>
       </c>
     </row>
     <row r="1875" spans="1:3">
       <c r="A1875" s="40"/>
-      <c r="C1875" s="34" t="s">
-        <v>2062</v>
-      </c>
+      <c r="C1875" s="84"/>
     </row>
     <row r="1876" spans="1:3">
       <c r="A1876" s="40"/>
-      <c r="C1876" s="56" t="s">
-        <v>2070</v>
+      <c r="C1876" s="84" t="s">
+        <v>2137</v>
       </c>
     </row>
     <row r="1877" spans="1:3">
       <c r="A1877" s="40"/>
-      <c r="C1877" s="56" t="s">
-        <v>2071</v>
+      <c r="C1877" s="84" t="s">
+        <v>2138</v>
       </c>
     </row>
     <row r="1878" spans="1:3">
       <c r="A1878" s="40"/>
-      <c r="C1878" s="56"/>
-    </row>
-    <row r="1879" spans="1:3">
-      <c r="A1879" s="40"/>
-      <c r="C1879" s="34" t="s">
-        <v>2063</v>
-      </c>
-    </row>
-    <row r="1880" spans="1:3">
-      <c r="A1880" s="40"/>
-      <c r="C1880" s="34" t="s">
-        <v>2064</v>
-      </c>
-    </row>
-    <row r="1881" spans="1:3">
-      <c r="A1881" s="40"/>
-      <c r="C1881" s="56" t="s">
-        <v>2072</v>
-      </c>
-    </row>
-    <row r="1882" spans="1:3">
-      <c r="A1882" s="40"/>
-      <c r="C1882" s="56" t="s">
-        <v>2073</v>
-      </c>
-    </row>
-    <row r="1883" spans="1:3">
-      <c r="A1883" s="40"/>
-      <c r="C1883" s="34" t="s">
-        <v>2065</v>
-      </c>
-    </row>
-    <row r="1884" spans="1:3">
-      <c r="A1884" s="40"/>
-      <c r="C1884" s="56" t="s">
-        <v>2074</v>
-      </c>
-    </row>
-    <row r="1885" spans="1:3">
-      <c r="A1885" s="40"/>
-      <c r="C1885" s="34" t="s">
-        <v>2066</v>
-      </c>
-    </row>
-    <row r="1886" spans="1:3" ht="30.5" customHeight="1">
-      <c r="A1886" s="40"/>
-      <c r="C1886" s="56" t="s">
-        <v>2075</v>
-      </c>
-    </row>
-    <row r="1887" spans="1:3">
-      <c r="A1887" s="40"/>
-      <c r="C1887" s="34"/>
-    </row>
-    <row r="1888" spans="1:3" ht="27">
-      <c r="A1888" s="40"/>
-      <c r="C1888" s="34" t="s">
-        <v>2076</v>
-      </c>
-    </row>
-    <row r="1889" spans="1:3">
-      <c r="A1889" s="40"/>
-      <c r="C1889" s="34"/>
-    </row>
-    <row r="1890" spans="1:3" ht="13" customHeight="1">
-      <c r="A1890" s="43"/>
-      <c r="B1890" s="92"/>
-      <c r="C1890" s="93"/>
+      <c r="C1878" s="34"/>
+    </row>
+    <row r="1879" spans="1:3" ht="13" customHeight="1">
+      <c r="A1879" s="43"/>
+      <c r="B1879" s="92"/>
+      <c r="C1879" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B1890:C1890"/>
+    <mergeCell ref="B1879:C1879"/>
     <mergeCell ref="A1590:C1590"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:C3"/>

</xml_diff>